<commit_message>
implemented jacoco and executable jars
</commit_message>
<xml_diff>
--- a/log-statistics.xlsx
+++ b/log-statistics.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>2019-06-16</t>
+    <t>2019-06-17</t>
   </si>
   <si>
     <t>RandomLogs</t>
@@ -112,7 +112,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -128,7 +128,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -136,7 +136,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
@@ -144,7 +144,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>